<commit_message>
incorporacion tabla resultados en excel
</commit_message>
<xml_diff>
--- a/back-end/MINEM.MIGI/MINEM.MIGI.Web/App_Data/PlantillaReporte.xlsx
+++ b/back-end/MINEM.MIGI/MINEM.MIGI.Web/App_Data/PlantillaReporte.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESCRITORIO\GIT MIGI\back-end\MINEM.MIGI\MINEM.MIGI.Web\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0642E54D-3FEF-47B8-B59C-5CCA361B349D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F3A9EF-AA7D-47FB-8A36-2E0FAE6C8087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3150" yWindow="1950" windowWidth="15840" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reporte" sheetId="1" r:id="rId1"/>
+    <sheet name="Reporte2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -339,7 +340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
@@ -347,4 +348,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EF73BB5-DDF8-4C96-A517-B3F015FF5B34}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>